<commit_message>
Create new env for tensorflow 📚🤓
</commit_message>
<xml_diff>
--- a/procesamiento de lenguaje natural/Act1/mia07_t3_tra_resultados_viterbi.xlsx
+++ b/procesamiento de lenguaje natural/Act1/mia07_t3_tra_resultados_viterbi.xlsx
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>DA0MS0</t>
+          <t>NCFS000</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -488,7 +488,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>2.779888150251198e-06</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -509,11 +509,11 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>NCFS000</t>
+          <t>VMIP3S0</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.0012941074971961</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -540,7 +540,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Fp</t>
+          <t>AQ0CS0</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -556,7 +556,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>6.385259012197449e-11</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -565,13 +565,13 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>3.529518322132861e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>NCMP000</t>
+          <t>DA0MS0</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -581,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>2.779888150251198e-06</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -593,7 +593,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>4.107075865754602e-15</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -602,11 +602,11 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>VMIP3S0</t>
+          <t>Fp</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0012941074971961</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -627,20 +627,20 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>3.529518322132861e-16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>AQ0CS0</t>
+          <t>SPS00</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1.988063133517315e-05</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -649,10 +649,10 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>6.385259012197449e-11</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>5.440257583147429e-12</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -664,7 +664,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>NCMS000</t>
+          <t>AQ0MS0</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -677,7 +677,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>2.827818374535177e-08</v>
+        <v>1.295582484193506e-09</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -695,14 +695,14 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>SPS00</t>
+          <t>NCMP000</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>1.988063133517315e-05</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -714,10 +714,10 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>5.440257583147429e-12</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>4.107075865754602e-15</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -726,7 +726,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>AQ0MS0</t>
+          <t>NCMS000</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -739,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>1.295582484193506e-09</v>
+        <v>2.827818374535177e-08</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>

</xml_diff>